<commit_message>
Added link type name as an attribute
</commit_message>
<xml_diff>
--- a/mtsim/examples/network_2_directed.xlsx
+++ b/mtsim/examples/network_2_directed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -159,6 +159,12 @@
     <t xml:space="preserve">BB</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">qmax</t>
   </si>
   <si>
@@ -198,10 +204,7 @@
     <t xml:space="preserve">node_to</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l</t>
+    <t xml:space="preserve">length</t>
   </si>
   <si>
     <t xml:space="preserve">count</t>
@@ -387,16 +390,16 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,7 +698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>30</v>
       </c>
@@ -703,6 +706,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C24" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="D24" s="0" t="s">
         <v>32</v>
       </c>
@@ -726,7 +732,7 @@
         <v>50248</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>31</v>
       </c>
@@ -734,6 +740,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C25" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="0" t="s">
         <v>33</v>
       </c>
@@ -757,7 +766,7 @@
         <v>15925</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>32</v>
       </c>
@@ -765,6 +774,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="D26" s="0" t="s">
         <v>34</v>
       </c>
@@ -788,7 +800,7 @@
         <v>18071</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>33</v>
       </c>
@@ -796,6 +808,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C27" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="D27" s="0" t="s">
         <v>35</v>
       </c>
@@ -819,7 +834,7 @@
         <v>14536</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>34</v>
       </c>
@@ -827,6 +842,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="D28" s="0" t="s">
         <v>36</v>
       </c>
@@ -850,7 +868,7 @@
         <v>20421</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>35</v>
       </c>
@@ -858,6 +876,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C29" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="D29" s="0" t="s">
         <v>37</v>
       </c>
@@ -881,7 +902,7 @@
         <v>12010</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>36</v>
       </c>
@@ -889,6 +910,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C30" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="D30" s="0" t="s">
         <v>38</v>
       </c>
@@ -912,7 +936,7 @@
         <v>7938</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>37</v>
       </c>
@@ -920,6 +944,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C31" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="D31" s="0" t="s">
         <v>39</v>
       </c>
@@ -943,7 +970,7 @@
         <v>13022</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>38</v>
       </c>
@@ -951,6 +978,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C32" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="D32" s="0" t="s">
         <v>40</v>
       </c>
@@ -974,7 +1004,7 @@
         <v>21497</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>39</v>
       </c>
@@ -982,6 +1012,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C33" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="D33" s="0" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +1038,7 @@
         <v>28211</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>40</v>
       </c>
@@ -1013,6 +1046,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C34" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="D34" s="0" t="s">
         <v>42</v>
       </c>
@@ -1036,13 +1072,16 @@
         <v>8859</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>41</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>43</v>
@@ -1085,30 +1124,30 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>70000</v>
+        <v>35000</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>110</v>
@@ -1136,10 +1175,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>125</v>
@@ -1156,10 +1195,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>90</v>
@@ -1176,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>80</v>
@@ -1196,10 +1235,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>15000</v>
+        <v>7500</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>65</v>
@@ -1216,10 +1255,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>15000</v>
+        <v>7500</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>50</v>
@@ -1236,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>40</v>
@@ -1272,10 +1311,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.15"/>
@@ -1287,22 +1326,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,10 +1361,10 @@
         <v>36</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>22542.5</v>
+        <v>22543</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,10 +1384,10 @@
         <v>36</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>22542.5</v>
+        <v>22543</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,10 +1407,10 @@
         <v>36.006</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>12567.5</v>
+        <v>12568</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,10 +1430,10 @@
         <v>36.006</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>12567.5</v>
+        <v>12568</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,7 +1453,7 @@
         <v>75.005</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>9544</v>
@@ -1437,7 +1476,7 @@
         <v>75.005</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>9544</v>
@@ -1460,7 +1499,7 @@
         <v>71.69</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>8640</v>
@@ -1483,7 +1522,7 @@
         <v>71.69</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>8640</v>
@@ -1506,7 +1545,7 @@
         <v>24.33</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>10098</v>
@@ -1529,7 +1568,7 @@
         <v>24.33</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>10098</v>
@@ -1552,10 +1591,10 @@
         <v>33.954</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>6233.5</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,10 +1614,10 @@
         <v>33.954</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>6233.5</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,7 +1637,7 @@
         <v>7.597</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>8902</v>
@@ -1621,7 +1660,7 @@
         <v>7.597</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>8902</v>
@@ -1644,7 +1683,7 @@
         <v>69.921</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>4085</v>
@@ -1667,7 +1706,7 @@
         <v>69.921</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>4085</v>
@@ -1690,7 +1729,7 @@
         <v>2.366</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>10370</v>
@@ -1713,7 +1752,7 @@
         <v>2.366</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>10370</v>
@@ -1736,10 +1775,10 @@
         <v>4.702</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>7377.5</v>
+        <v>7378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,10 +1798,10 @@
         <v>4.702</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>7377.5</v>
+        <v>7378</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,10 +1821,10 @@
         <v>28.518</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>7864.5</v>
+        <v>7865</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,10 +1844,10 @@
         <v>28.518</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>7864.5</v>
+        <v>7865</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,10 +1867,10 @@
         <v>11.595</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>6558.5</v>
+        <v>6559</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,10 +1890,10 @@
         <v>11.595</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>6558.5</v>
+        <v>6559</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,10 +1913,10 @@
         <v>87.491</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>8697.5</v>
+        <v>8698</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,10 +1936,10 @@
         <v>87.491</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>8697.5</v>
+        <v>8698</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,10 +1959,10 @@
         <v>5.349</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>6992.5</v>
+        <v>6993</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,10 +1982,10 @@
         <v>5.349</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>6992.5</v>
+        <v>6993</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +2005,7 @@
         <v>14.296</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>10792</v>
@@ -1989,7 +2028,7 @@
         <v>14.296</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>10792</v>
@@ -2012,7 +2051,7 @@
         <v>2.375</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>12831</v>
@@ -2035,7 +2074,7 @@
         <v>2.375</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>12831</v>
@@ -2058,7 +2097,7 @@
         <v>4.59</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>5796</v>
@@ -2081,7 +2120,7 @@
         <v>4.59</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>5796</v>
@@ -2104,7 +2143,7 @@
         <v>7.123</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>7315</v>
@@ -2127,7 +2166,7 @@
         <v>7.123</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>7315</v>
@@ -2150,10 +2189,10 @@
         <v>48.731</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>3849.5</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,10 +2212,10 @@
         <v>48.731</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>3849.5</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2235,7 @@
         <v>191.308</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>3583</v>
@@ -2219,7 +2258,7 @@
         <v>191.308</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>3583</v>
@@ -2242,10 +2281,10 @@
         <v>8.233</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>15213.5</v>
+        <v>15214</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,10 +2304,10 @@
         <v>8.233</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>15213.5</v>
+        <v>15214</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,10 +2327,10 @@
         <v>40.261</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>5545.5</v>
+        <v>5546</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,10 +2350,10 @@
         <v>40.261</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>5545.5</v>
+        <v>5546</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,7 +2373,7 @@
         <v>29.173</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>5961</v>
@@ -2357,7 +2396,7 @@
         <v>29.173</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>5961</v>
@@ -2380,10 +2419,10 @@
         <v>67.4</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>1359.5</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,10 +2442,10 @@
         <v>67.4</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>1359.5</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2465,7 @@
         <v>10.036</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,6 +2483,9 @@
       </c>
       <c r="E51" s="0" t="n">
         <v>10.036</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>